<commit_message>
added VOL+Weight to xlsx for copying
Finded out, that I missed total volume and weight in the excel format used for copying so I included it
</commit_message>
<xml_diff>
--- a/vol2.xlsx
+++ b/vol2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,23 +436,109 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Volume</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Weight [4]</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>----</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>----</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>len_Wi_Hei_Wei_Pack</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="B2" t="n">
+        <v>12</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>2x  40x50x60 cm  12 kg/ctn</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2x  80x98x100 cm  120 kg/plt</t>
-        </is>
-      </c>
+      <c r="A3" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="B3" t="n">
+        <v>17</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>12x  50x15x60 cm  17 kg/ctn</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>6.2208</v>
+      </c>
+      <c r="B4" t="n">
+        <v>50</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>54x  120x80x12 cm  50 kg/plt</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>7.0008</v>
+      </c>
+      <c r="B5" t="n">
+        <v>79</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>